<commit_message>
Qi Update - removed awards, updated directory
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24420" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20980" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="979">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2931,6 +2931,39 @@
   </si>
   <si>
     <t>One woman&amp;rsquo;s life told through fragments of time that stretch over four decades.</t>
+  </si>
+  <si>
+    <t>Rue Sparks</t>
+  </si>
+  <si>
+    <t>Speculative, Magical Realism, SFF</t>
+  </si>
+  <si>
+    <t>Daylight Chasers</t>
+  </si>
+  <si>
+    <t>https://linktr.ee/ruesparks</t>
+  </si>
+  <si>
+    <t>During a time-zone-hopping road trip, a client&amp;rsquo;s mercurial moods and thinly veiled secret leaves Keenan wondering: how can he be the guide when even he is feeling lost?</t>
+  </si>
+  <si>
+    <t>@sparks_writes</t>
+  </si>
+  <si>
+    <t>Miles Nelson</t>
+  </si>
+  <si>
+    <t>Riftmaster</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Riftmaster-Miles-Nelson-ebook/dp/B08WJGPY3W/</t>
+  </si>
+  <si>
+    <t>College student bailey jones is wrenched away from earth by a mysterious and unpredictable force known as the Rift. While stranded on an alien planet, he meets a mysterious traveller known as the Riftmaster.</t>
+  </si>
+  <si>
+    <t>@ProbablyMiles</t>
   </si>
 </sst>
 </file>
@@ -3264,11 +3297,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L166"/>
+  <dimension ref="A1:L168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G165" sqref="G165"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I169" sqref="I169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8061,7 +8094,7 @@
         <v>768</v>
       </c>
       <c r="I133" s="15" t="str">
-        <f t="shared" ref="I133:I166" si="2">"["&amp;CHAR(39)&amp;C133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;F133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;E133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;D133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;H133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;G133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;J133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;K133&amp;CHAR(39)&amp;"],"</f>
+        <f t="shared" ref="I133:I168" si="2">"["&amp;CHAR(39)&amp;C133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;F133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;E133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;D133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;H133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;G133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;J133&amp;CHAR(39)&amp;","&amp;CHAR(39)&amp;K133&amp;CHAR(39)&amp;"],"</f>
         <v>['Gabriel Constans','https://www.amazon.com/Last-Conception-Gabriel-Constans-ebook/dp/B00LVGZO3U/','The Last Conception','LesFic','@GabrielConstans','Her parents tell Savarna she MUST have a baby because she&amp;rsquo;s the last in succession of a spiritual teacher followed by millions.  She doesn&amp;rsquo;t believe it. Her girlfriend does.','genre-love','age-adult'],</v>
       </c>
       <c r="J133" s="15" t="s">
@@ -9256,6 +9289,78 @@
         <v>186</v>
       </c>
       <c r="K166" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A167" s="1">
+        <v>44253.887003136573</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="G167" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="I167" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v>['Rue Sparks','https://linktr.ee/ruesparks','Daylight Chasers','Speculative, Magical Realism, SFF','@sparks_writes','During a time-zone-hopping road trip, a client&amp;rsquo;s mercurial moods and thinly veiled secret leaves Keenan wondering: how can he be the guide when even he is feeling lost?','genre-speculative','age-adult'],</v>
+      </c>
+      <c r="J167" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="K167" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A168" s="1">
+        <v>44264.16777443287</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="G168" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="H168" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="I168" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v>['Miles Nelson','https://www.amazon.com/Riftmaster-Miles-Nelson-ebook/dp/B08WJGPY3W/','Riftmaster','Science Fiction','@ProbablyMiles','College student bailey jones is wrenched away from earth by a mysterious and unpredictable force known as the Rift. While stranded on an alien planet, he meets a mysterious traveller known as the Riftmaster.','genre-speculative','age-adult'],</v>
+      </c>
+      <c r="J168" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="K168" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -9419,6 +9524,8 @@
     <hyperlink ref="F163" r:id="rId155"/>
     <hyperlink ref="F164" r:id="rId156"/>
     <hyperlink ref="F166" r:id="rId157"/>
+    <hyperlink ref="F167" r:id="rId158"/>
+    <hyperlink ref="F168" r:id="rId159"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>